<commit_message>
added new data row
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Data2 2.xlsx
+++ b/src/test/resources/testdata/Data2 2.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saniyatairova/IdeaProjects/MindtekCucumberFramework/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B3706C-A87C-4646-99A8-A1470E0A5EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA49E6B7-71A8-DE42-A081-DF002642CF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{594ADE93-3FEA-7A45-BC2F-519BC6BA9803}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>firstName</t>
   </si>
@@ -65,20 +65,25 @@
     <t>321 Strings Dr, Kenosha WI</t>
   </si>
   <si>
-    <t>Springs</t>
-  </si>
-  <si>
-    <t>Smile</t>
-  </si>
-  <si>
     <t>Kevin</t>
+  </si>
+  <si>
+    <t>smith</t>
+  </si>
+  <si>
+    <t>com</t>
+  </si>
+  <si>
+    <t>skdjfskdjfsdkfjds</t>
+  </si>
+  <si>
+    <t>dfsjdfosijdfsl sdfjsdkj sdfjl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -435,16 +440,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4AD08F8-E6A0-D141-B390-473E55C0B4B1}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="19.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.83203125" collapsed="true"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -480,13 +485,27 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more Data added for "iD" cell
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Data2 2.xlsx
+++ b/src/test/resources/testdata/Data2 2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saniyatairova/IdeaProjects/MindtekCucumberFramework/src/test/resources/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saniyatairova/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA49E6B7-71A8-DE42-A081-DF002642CF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{597B6654-EA0A-8F4F-A891-4EC8C6378531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{594ADE93-3FEA-7A45-BC2F-519BC6BA9803}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>firstName</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>dfsjdfosijdfsl sdfjsdkj sdfjl</t>
+  </si>
+  <si>
+    <t>iD</t>
   </si>
 </sst>
 </file>
@@ -440,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4AD08F8-E6A0-D141-B390-473E55C0B4B1}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -452,7 +455,7 @@
     <col min="4" max="4" width="23.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,8 +468,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -479,8 +485,11 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
+      <c r="E2">
+        <v>232</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -493,8 +502,11 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
+      <c r="E3">
+        <v>233</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -506,6 +518,9 @@
       </c>
       <c r="D4" t="s">
         <v>14</v>
+      </c>
+      <c r="E4">
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>